<commit_message>
rust occurence counter implemented
</commit_message>
<xml_diff>
--- a/resumes.xlsx
+++ b/resumes.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,1842 @@
       <c r="B1" t="inlineStr">
         <is>
           <t>Keywords</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Adebiyi, Adesina_Oliver - 2023-05-31 19-37-42.docx</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Team, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Adetifa, Olaniyi - 2023-03-21 19-53-54.pdf</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Agoun, Mostefa - 2023-03-26 02-33-47.pdf</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Ajanaku, Kenny - 2023-03-21 17-44-33.docx</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Akile, Emmanuel - 2023-03-21 23-57-37.pdf</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Al-Amad, Farouq - 2023-03-22 01-01-23.pdf</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Algharbawy_(PMP)__, Ahmed - 2023-05-19 23-23-53.pdf</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Almeida, Bruno - 2023-05-31 19-35-55.pdf</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Team, SQL, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Alnawasrah, Sharaf - 2023-05-21 22-34-11.pdf</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Team, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Amirtharaj, Asha - 2023-03-24 10-30-19.docx</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Anurag_Kuri, James - 2023-03-24 12-00-50.docx</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Team, Python, SQL, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Avanesyan, Davit - 2023-06-07 11-06-19.docx</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>BANTWAL, MANJUNATHA - 2023-05-23 12-28-42.pdf</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>BOROLE, SHAILESH - 2023-03-23 09-49-59.pdf</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Balkan, Batin_Can - 2023-05-17 21-50-43.pdf</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Balkan, Batin_Can - 2023-05-22 23-15-05.pdf</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Barbosa, Cec__lia - 2023-03-21 01-36-26.pdf</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Team, Python, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Bayoumi, Sherif - 2023-05-24 21-20-03.pdf</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Bergstrom__PMP, Neeva - 2023-05-31 17-51-29.pdf</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Bhavan, Shehan - 2023-05-03 17-23-47.pdf</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Python, SQL, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Biodun-oyedepo, Tolu - 2023-03-29 19-59-19.pdf</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Blair, Geoffrey - 2018-03-16 16-17-28.docx</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Team, SQL, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Bunce, Matt - 2022-09-19 22-24-47.pdf</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Team, Python, HTML, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Butala, Harsh - 2023-05-20 12-42-18.pdf</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Chigarev, Evgeny - 2023-04-10 07-25-37.pdf</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Chopra, Karan - 2023-05-12 01-57-04.pdf</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Javascript, SQL, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Christian, Ajukwu - 2023-03-27 18-11-35.docx</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Team, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Coles, Bruce - 2023-05-08 22-59-26.pdf</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Team, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Colquhoun, Sreedevi - 2023-03-28 16-55-04.pdf</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Costa, Eduardo - 2023-04-05 17-43-58.pdf</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Team, SQL, HTML, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>DHAWAN, PRIYANK - 2023-03-20 23-25-47.docx</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Dave, Jaydeep - 2023-03-21 19-28-27.pdf</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Team, Javascript, SQL, HTML, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Davidson, Cortland - 2023-03-22 16-44-32.pdf</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Team, Python, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Del_Cid, Jaime - 2023-06-07 01-06-58.pdf</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Dewani, Vishesh - 2023-03-23 07-05-15.pdf</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Team, SQL, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Dey, Alakananda - 2023-06-03 19-00-03.pdf</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Elbagoury, Mohamed - 2023-05-02 17-16-05.pdf</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Elsirfy, Tamer - 2023-05-19 06-06-23.pdf</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Team, Javascript, SQL, HTML, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Emore, Efe - 2023-06-05 04-51-37.docx</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Team, Diploma, SQL, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Farooqi__PMP__Prince2, Wasif - 2023-05-08 20-46-16.pdf</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Farooqi__PMP__Prince2, Wasif - 2023-06-08 15-13-36.pdf</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>GANADHI, VANITHA - 2023-03-23 13-39-23.docx</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>GHODKE, VIPIN - 2023-04-17 13-10-55.docx</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>GUPTA, NATASHA - 2023-03-27 09-54-59.pdf</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Team, Python, Javascript, HTML, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Gawli, Komal - 2023-04-28 15-47-21.pdf</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Ghulam_Murtza, Malik - 2023-05-29 06-13-10.pdf</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Team, SQL, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Gonsalves, Serafin - 2023-04-17 19-01-08.docx</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Gu, Daniel - 2023-06-05 16-07-26.pdf</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Team, Python, SQL, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Gu, Daniel - 2023-06-06 17-00-15.pdf</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Team, Python, SQL, HTML, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Gu, huaien - 2023-05-31 19-05-09.pdf</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Team, Python, SQL, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Gubanov, Aleksei - 2023-05-10 16-27-27.pdf</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Team, SQL, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Gulam, Mohammed_Yawar - 2023-05-12 23-09-41.pdf</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Team, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Gupta, Rahul - 2023-03-22 17-37-14.pdf</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Team, Python, SQL, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Hamarsha, Mahmoud - 2023-05-20 18-21-29.docx</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Hamdy, Ali - 2023-06-04 09-04-30.pdf</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Hervas, Mauricio - 2022-09-22 20-16-06.docx</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Diploma, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Ilunga, Bebel - 2023-05-24 22-03-57.pdf</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Javascript, HTML, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Isemede, Daniel - 2023-04-12 02-18-56.pdf</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>KAUL, VISHESH - 2023-03-30 13-19-02.pdf</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>KHAN, IMRAN - 2023-04-15 01-02-25.pdf</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>KOTEESWARAN, V.P. - 2023-05-30 17-15-21.pdf</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Diploma, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Kapoor__PSM_1__PMP____MBA__MCA, Gaurav - 2023-04-17 21-49-11.docx</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Keen, Jeff - 2023-04-17 17-52-45.pdf</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Team, Javascript, SQL, HTML, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Khalid, Imran - 2023-03-22 07-11-40.pdf</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Team, Python, SQL, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Khan, Mohammed_Ashfaqullah - 2023-05-23 17-39-49.pdf</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Team, SQL, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Khoday, Greta - 2023-06-01 17-38-32.pdf</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Khublani, Penjani - 2023-03-27 17-15-24.pdf</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Team, SQL, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Kostiuchenko, Andrii - 2023-03-31 21-00-27.pdf</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Team, SQL, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Kovaloff, Tratham - 2023-03-29 02-24-44.pdf</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Kuffar, Hendrika - 2023-03-27 04-05-48.pdf</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Team, Python, Javascript, SQL, HTML, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Kumar, surjit - 2023-04-14 04-20-06.docx</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Kuppusamy, Vijayakumar - 2023-04-21 16-24-07.pdf</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Team, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Luu, Van - 2023-06-05 16-05-10.docx</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>MOORJANI, RAJESH - 2023-04-15 07-04-14.docx</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>MOORJANI, RAJESH - 2023-05-20 10-21-32.pdf</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Madaan, Rajat - 2023-03-28 21-10-34.pdf</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Team, Diploma, SQL, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Madhukar, Shashikiran - 2023-04-12 06-11-11.pdf</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Team, SQL, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Mahajan, Indrajit - 2023-03-22 02-50-08.pdf</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Team, SQL, HTML, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Marzoque, William - 2023-03-24 01-56-03.pdf</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Javascript, SQL, HTML, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Mathur, Mohak - 2023-06-07 14-16-09.pdf</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Megalingam, Murali - 2023-05-16 10-30-37.docx</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Team, Python, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Metawala, Paras - 2023-06-05 10-49-55.pdf</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Javascript, SQL, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Mohammed, Viquar - 2023-03-21 02-26-38.pdf</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Team, Javascript, SQL, HTML, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Montgomery-Andersen, Stephan - 2023-06-05 04-20-21.pdf</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Mundada_Inani, Namita - 2023-03-21 15-44-23.pdf</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Murthy, Vishal - 2023-03-26 09-16-31.docx</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Myronenko, Eugene - 2023-05-26 14-00-03.docx</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Narasingam_Kuppusamy, Vijayakumar - 2023-04-19 02-10-13.pdf</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Team, SQL, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Navrotsky, Michael - 2023-06-06 14-53-32.pdf</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Team, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Neil, Ulka - 2023-03-28 08-43-34.pdf</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Nigam, Akash - 2023-05-22 11-56-33.pdf</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Team, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>OLAJIDE, PETER - 2023-03-21 19-17-22.pdf</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Team, Python, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Oketokun, Joseph - 2023-04-08 18-04-19.docx</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Onyschtschuk, Peter - 2023-06-05 17-36-43.docx</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Palyam, Rakesh - 2023-05-09 04-12-31.pdf</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Team, Python, Javascript, SQL, HTML, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Pascal_Yvon, MAYANG_Fokou - 2023-04-29 21-55-56.pdf</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Patel, Jaydeep - 2023-06-02 16-36-33.pdf</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Javascript, SQL, HTML, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Patil, Sneha - 2023-05-21 02-17-24.pdf</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Pavlenko, Alexey - 2023-06-06 22-01-58.pdf</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Team, Javascript, SQL, HTML, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Pednekar_-_PMP_OCP_MCA, Sumit - 2023-06-05 18-22-41.docx</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Pereira, Ana - 2023-05-23 03-17-43.pdf</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Pereira, Ana - 2023-05-28 23-10-24.pdf</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Pinto, Bruno - 2023-05-26 13-49-36.pdf</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Pmp, Ross - 2023-04-05 02-18-37.docx</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Team, SQL, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Pulak, Greg - 2023-03-21 23-44-56.pdf</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Ragab, Eman - 2023-04-27 12-19-15.pdf</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Raghav_, Kirti - 2023-05-10 13-53-49.pdf</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Javascript, SQL, HTML, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Raghav_, Kirti - 2023-05-24 07-04-34.pdf</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Javascript, SQL, HTML, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Raju, Robin - 2023-06-04 15-19-57.pdf</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Rani, Sapna - 2023-04-04 12-12-19.pdf</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Rao, Ramesh - 2023-05-31 04-40-53.pdf</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Raza, Muhammad_Tahir - 2023-06-02 09-14-02.docx</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Refaei, Mohamed - 2023-03-21 15-34-41.pdf</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Relekar, Sunita - 2023-05-24 05-12-59.docx</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Reshetnyak, Yuriy - 2023-05-12 22-12-31.pdf</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Team, SQL, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Richard, Mark - 2023-05-30 17-37-58.pdf</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Rupawala, Hozefa - 2023-05-16 12-42-32.pdf</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>SHAIKH, SHAKIR - 2023-03-21 07-03-04.pdf</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>SHARMA, MOHIT - 2023-04-01 21-59-29.pdf</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Team, Python, Javascript, SQL, HTML, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>SINGH, KAJAL - 2023-05-17 10-28-51.docx</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>SYUNRY, PRASHANT - 2023-03-30 17-57-09.pdf</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Team, SQL, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>S_G, Greeshma - 2023-06-05 03-28-01.docx</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Team, Python, SQL, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>S_Shamaa, Firas - 2023-03-31 13-18-33.pdf</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Saluja, Mahendra - 2023-04-02 15-45-22.pdf</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Sankaran, Vijayaraaghavan - 2023-06-02 07-26-26.pdf</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Team, Diploma, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Saraf, Ajay - 2023-05-28 17-28-19.pdf</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Schotborgh, Cesar - 2023-03-22 14-52-58.pdf</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Scott-simpson, Shannon - 2023-05-10 21-46-28.pdf</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Team, Python, Javascript, SQL, HTML, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Shah, Chintan - 2023-06-04 14-30-28.pdf</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Team, Python, Javascript, SQL, HTML, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Shama, Emad - 2023-04-12 19-45-02.pdf</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Shama, Firas - 2023-03-31 13-22-25.pdf</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Sharma, Prashant - 2023-04-18 20-57-15.pdf</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Team, Diploma, SQL, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Sharma, Rahul - 2023-03-23 16-41-57.pdf</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Javascript, SQL, HTML, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Singh, Avinash - 2023-05-25 07-48-30.pdf</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Team, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Sleeman, Richard - 2023-03-27 11-24-59.pdf</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Somatillaka, Jayan - 2023-03-21 22-03-43.pdf</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Python, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Somatillaka, Jayan - 2023-03-23 16-59-26.pdf</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Python, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Somatillaka, Jayan - 2023-05-28 19-43-01.pdf</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Python, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Sushila, s - 2023-04-02 13-25-02.pdf</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Sutar, Hemant - 2023-05-04 02-43-44.pdf</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Tripuraneni, Nandana - 2023-06-01 14-14-40.docx</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Team, Javascript, SQL, HTML, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Ukwu, Chinedu - 2023-03-28 19-44-48.pdf</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Team, SQL, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>V, ShanthaMoorthy - 2023-05-17 10-05-39.pdf</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>V.P, Thiruvengadavan - 2023-05-14 04-16-47.pdf</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Velasquez, Gil - 2023-05-24 15-43-48.docx</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Team, SQL, HTML, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Vemuri, John - 2023-04-04 18-23-21.docx</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Vijayan, Sajiv - 2023-03-26 10-09-24.docx</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Team, SQL, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Vinodh_Kumar, Krishna_Priya - 2023-04-11 09-30-52.docx</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Team, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Wagar, Daeton - 2023-04-25 20-21-17.docx</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Team, Oracle, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Walters, Delano - 2023-06-05 10-31-38.docx</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Wilson, Gloria - 2018-02-26 18-19-13.docx</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Team, Diploma, SQL, HTML, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Win, Kyi_Kyi - 2023-05-31 05-40-41.pdf</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Team, Diploma, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Yadua_, Gabriel - 2023-03-21 01-45-48.pdf</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Yalcinoz, Gorkem - 2023-03-20 22-53-07.pdf</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Team, Python, Javascript, SQL, HTML, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Younas, Naveedn - 2023-05-24 02-02-03.pdf</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Team, SQL, Oracle, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>bhatia, Aanchal_ - 2023-06-01 07-44-23.pdf</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Team, SQL, Manage, Admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>kaul, vishesh - 2023-04-17 08-38-00.pdf</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Team, Manage</t>
         </is>
       </c>
     </row>

</xml_diff>